<commit_message>
Form submissions now map to proper cell, including merged columns
</commit_message>
<xml_diff>
--- a/base_template.xlsx
+++ b/base_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmckenzie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmckenzie/Desktop/Avalon NEWEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2815C-8C6D-2F40-ADC3-A2699C502BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AFB68A-469C-E14E-898D-42717C9F18E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="2" xr2:uid="{98C021A7-547A-C84F-B88C-65745982F461}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="2" xr2:uid="{98C021A7-547A-C84F-B88C-65745982F461}"/>
   </bookViews>
   <sheets>
     <sheet name="Roll Up Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="106">
   <si>
     <t>Production Month:</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>psi Hyd</t>
+  </si>
+  <si>
+    <t>Oil (m3)</t>
   </si>
 </sst>
 </file>
@@ -2177,6 +2180,21 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2199,6 +2217,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2213,32 +2267,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2251,78 +2279,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="2" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="2" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3649,25 +3652,25 @@
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="244" t="s">
+      <c r="D5" s="249" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="245"/>
-      <c r="F5" s="245"/>
-      <c r="G5" s="245"/>
-      <c r="H5" s="246"/>
-      <c r="I5" s="247" t="s">
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="250"/>
+      <c r="H5" s="251"/>
+      <c r="I5" s="252" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="250" t="s">
+      <c r="J5" s="255" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="251"/>
-      <c r="L5" s="252"/>
-      <c r="M5" s="256" t="s">
+      <c r="K5" s="256"/>
+      <c r="L5" s="257"/>
+      <c r="M5" s="261" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="247" t="s">
+      <c r="N5" s="252" t="s">
         <v>5</v>
       </c>
       <c r="O5" s="11"/>
@@ -3717,12 +3720,12 @@
       <c r="H6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="248"/>
-      <c r="J6" s="253"/>
-      <c r="K6" s="254"/>
-      <c r="L6" s="255"/>
-      <c r="M6" s="257"/>
-      <c r="N6" s="248"/>
+      <c r="I6" s="253"/>
+      <c r="J6" s="258"/>
+      <c r="K6" s="259"/>
+      <c r="L6" s="260"/>
+      <c r="M6" s="262"/>
+      <c r="N6" s="253"/>
       <c r="O6" s="13" t="s">
         <v>12</v>
       </c>
@@ -3770,7 +3773,7 @@
       <c r="H7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="249"/>
+      <c r="I7" s="254"/>
       <c r="J7" s="24" t="s">
         <v>17</v>
       </c>
@@ -3780,8 +3783,8 @@
       <c r="L7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="255"/>
-      <c r="N7" s="249"/>
+      <c r="M7" s="260"/>
+      <c r="N7" s="254"/>
       <c r="O7" s="26"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
@@ -10445,7 +10448,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M6" sqref="M6"/>
+      <selection pane="topRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10765,109 +10768,109 @@
       <c r="BM4" s="45"/>
     </row>
     <row r="5" spans="1:65" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="284" t="s">
+      <c r="A5" s="265" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="285" t="s">
+      <c r="B5" s="273" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="285" t="s">
+      <c r="C5" s="273" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="284" t="s">
+      <c r="D5" s="265" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="284" t="s">
+      <c r="E5" s="265" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="284" t="s">
+      <c r="F5" s="265" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="284" t="s">
+      <c r="G5" s="265" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="286" t="s">
+      <c r="H5" s="269" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="286" t="s">
+      <c r="I5" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="286" t="s">
+      <c r="J5" s="269" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="286" t="s">
+      <c r="K5" s="269" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="286" t="s">
+      <c r="L5" s="269" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="277" t="s">
+      <c r="M5" s="280" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="278"/>
-      <c r="O5" s="278"/>
-      <c r="P5" s="278"/>
-      <c r="Q5" s="278"/>
-      <c r="R5" s="278"/>
-      <c r="S5" s="284" t="s">
+      <c r="N5" s="281"/>
+      <c r="O5" s="281"/>
+      <c r="P5" s="281"/>
+      <c r="Q5" s="281"/>
+      <c r="R5" s="281"/>
+      <c r="S5" s="265" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="294" t="s">
+      <c r="T5" s="288" t="s">
         <v>97</v>
       </c>
-      <c r="U5" s="295" t="s">
+      <c r="U5" s="290" t="s">
         <v>98</v>
       </c>
-      <c r="V5" s="286" t="s">
+      <c r="V5" s="269" t="s">
         <v>99</v>
       </c>
-      <c r="W5" s="279" t="s">
+      <c r="W5" s="282" t="s">
         <v>32</v>
       </c>
-      <c r="X5" s="280"/>
-      <c r="Y5" s="301" t="s">
+      <c r="X5" s="283"/>
+      <c r="Y5" s="271" t="s">
         <v>100</v>
       </c>
-      <c r="Z5" s="284" t="s">
+      <c r="Z5" s="265" t="s">
         <v>101</v>
       </c>
-      <c r="AA5" s="284" t="s">
+      <c r="AA5" s="265" t="s">
         <v>102</v>
       </c>
-      <c r="AB5" s="284" t="s">
+      <c r="AB5" s="265" t="s">
         <v>103</v>
       </c>
-      <c r="AC5" s="302" t="s">
+      <c r="AC5" s="263" t="s">
         <v>40</v>
       </c>
-      <c r="AD5" s="284" t="s">
+      <c r="AD5" s="265" t="s">
         <v>104</v>
       </c>
-      <c r="AE5" s="284" t="s">
+      <c r="AE5" s="265" t="s">
         <v>33</v>
       </c>
-      <c r="AF5" s="264" t="s">
+      <c r="AF5" s="284" t="s">
         <v>55</v>
       </c>
-      <c r="AG5" s="282" t="s">
+      <c r="AG5" s="267" t="s">
         <v>57</v>
       </c>
-      <c r="AH5" s="258" t="s">
+      <c r="AH5" s="275" t="s">
         <v>34</v>
       </c>
-      <c r="AI5" s="259"/>
-      <c r="AJ5" s="259"/>
-      <c r="AK5" s="259"/>
-      <c r="AL5" s="259"/>
-      <c r="AM5" s="260"/>
-      <c r="AN5" s="258" t="s">
+      <c r="AI5" s="276"/>
+      <c r="AJ5" s="276"/>
+      <c r="AK5" s="276"/>
+      <c r="AL5" s="276"/>
+      <c r="AM5" s="277"/>
+      <c r="AN5" s="275" t="s">
         <v>56</v>
       </c>
-      <c r="AO5" s="259"/>
-      <c r="AP5" s="259"/>
-      <c r="AQ5" s="259"/>
-      <c r="AR5" s="259"/>
-      <c r="AS5" s="260"/>
+      <c r="AO5" s="276"/>
+      <c r="AP5" s="276"/>
+      <c r="AQ5" s="276"/>
+      <c r="AR5" s="276"/>
+      <c r="AS5" s="277"/>
       <c r="AT5" s="55"/>
       <c r="AU5" s="55"/>
       <c r="AV5" s="55"/>
@@ -10890,55 +10893,55 @@
       <c r="BM5" s="55"/>
     </row>
     <row r="6" spans="1:65" ht="25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="287"/>
-      <c r="B6" s="288"/>
-      <c r="C6" s="288"/>
-      <c r="D6" s="287"/>
-      <c r="E6" s="287"/>
-      <c r="F6" s="287"/>
-      <c r="G6" s="287"/>
-      <c r="H6" s="289"/>
-      <c r="I6" s="289"/>
-      <c r="J6" s="289"/>
-      <c r="K6" s="289"/>
-      <c r="L6" s="290"/>
+      <c r="A6" s="266"/>
+      <c r="B6" s="274"/>
+      <c r="C6" s="274"/>
+      <c r="D6" s="266"/>
+      <c r="E6" s="266"/>
+      <c r="F6" s="266"/>
+      <c r="G6" s="266"/>
+      <c r="H6" s="270"/>
+      <c r="I6" s="270"/>
+      <c r="J6" s="270"/>
+      <c r="K6" s="270"/>
+      <c r="L6" s="286"/>
       <c r="M6" s="56" t="s">
         <v>36</v>
       </c>
       <c r="N6" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="291" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="291" t="s">
+      <c r="O6" s="244" t="s">
+        <v>105</v>
+      </c>
+      <c r="P6" s="244" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="292" t="s">
+      <c r="Q6" s="245" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="293" t="s">
+      <c r="R6" s="246" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="296"/>
-      <c r="T6" s="297"/>
-      <c r="U6" s="298"/>
-      <c r="V6" s="289"/>
-      <c r="W6" s="299" t="s">
+      <c r="S6" s="287"/>
+      <c r="T6" s="289"/>
+      <c r="U6" s="291"/>
+      <c r="V6" s="270"/>
+      <c r="W6" s="247" t="s">
         <v>38</v>
       </c>
-      <c r="X6" s="300" t="s">
+      <c r="X6" s="248" t="s">
         <v>39</v>
       </c>
-      <c r="Y6" s="303"/>
-      <c r="Z6" s="287"/>
-      <c r="AA6" s="287"/>
-      <c r="AB6" s="287"/>
-      <c r="AC6" s="304"/>
-      <c r="AD6" s="287"/>
-      <c r="AE6" s="287"/>
-      <c r="AF6" s="281"/>
-      <c r="AG6" s="283"/>
+      <c r="Y6" s="272"/>
+      <c r="Z6" s="266"/>
+      <c r="AA6" s="266"/>
+      <c r="AB6" s="266"/>
+      <c r="AC6" s="264"/>
+      <c r="AD6" s="266"/>
+      <c r="AE6" s="266"/>
+      <c r="AF6" s="285"/>
+      <c r="AG6" s="268"/>
       <c r="AH6" s="228" t="s">
         <v>41</v>
       </c>
@@ -13706,11 +13709,11 @@
     </row>
     <row r="40" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="42"/>
-      <c r="B40" s="261" t="s">
+      <c r="B40" s="278" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="262"/>
-      <c r="D40" s="262"/>
+      <c r="C40" s="279"/>
+      <c r="D40" s="279"/>
       <c r="E40" s="197"/>
       <c r="F40" s="198" t="s">
         <v>21</v>
@@ -28213,20 +28216,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AG5:AG6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB5:AB6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
     <mergeCell ref="AN5:AS5"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="M5:R5"/>
@@ -28243,6 +28232,20 @@
     <mergeCell ref="S5:S6"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="U5:U6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AB6"/>
   </mergeCells>
   <dataValidations xWindow="80" yWindow="499" count="4">
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" prompt="INPUT TICKET NUMBER - Please input the ticket number. Use &quot;/&quot; to separate multiple ticket numbers." sqref="T15:T37 U7:U37 Q7:R37 T7 T9:T13" xr:uid="{E0AF0162-8FCD-CE4D-A844-6D6A6F47490E}">
@@ -28309,13 +28312,13 @@
       <c r="F1" s="172" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="275" t="s">
+      <c r="G1" s="297" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="276"/>
-      <c r="I1" s="276"/>
-      <c r="J1" s="276"/>
-      <c r="K1" s="263"/>
+      <c r="H1" s="298"/>
+      <c r="I1" s="298"/>
+      <c r="J1" s="298"/>
+      <c r="K1" s="299"/>
       <c r="L1" s="173"/>
       <c r="M1" s="102" t="s">
         <v>63</v>
@@ -28336,18 +28339,18 @@
         <v>68</v>
       </c>
       <c r="S1" s="173"/>
-      <c r="T1" s="271" t="s">
+      <c r="T1" s="292" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="271"/>
-      <c r="V1" s="271"/>
+      <c r="U1" s="292"/>
+      <c r="V1" s="292"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="272" t="s">
+      <c r="X1" s="293" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="262"/>
-      <c r="Z1" s="262"/>
-      <c r="AA1" s="262"/>
+      <c r="Y1" s="279"/>
+      <c r="Z1" s="279"/>
+      <c r="AA1" s="279"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="173"/>
       <c r="AD1" s="173"/>
@@ -28411,11 +28414,11 @@
       <c r="D3" s="102"/>
       <c r="E3" s="185"/>
       <c r="F3" s="185"/>
-      <c r="G3" s="268"/>
-      <c r="H3" s="273"/>
-      <c r="I3" s="273"/>
-      <c r="J3" s="273"/>
-      <c r="K3" s="274"/>
+      <c r="G3" s="294"/>
+      <c r="H3" s="295"/>
+      <c r="I3" s="295"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="296"/>
       <c r="L3" s="173"/>
       <c r="M3" s="173">
         <v>1</v>
@@ -28453,11 +28456,11 @@
       <c r="D4" s="102"/>
       <c r="E4" s="185"/>
       <c r="F4" s="185"/>
-      <c r="G4" s="268"/>
-      <c r="H4" s="273"/>
-      <c r="I4" s="273"/>
-      <c r="J4" s="273"/>
-      <c r="K4" s="274"/>
+      <c r="G4" s="294"/>
+      <c r="H4" s="295"/>
+      <c r="I4" s="295"/>
+      <c r="J4" s="295"/>
+      <c r="K4" s="296"/>
       <c r="L4" s="173"/>
       <c r="M4" s="173">
         <v>2</v>
@@ -28495,11 +28498,11 @@
       <c r="D5" s="187"/>
       <c r="E5" s="185"/>
       <c r="F5" s="185"/>
-      <c r="G5" s="268"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="274"/>
+      <c r="G5" s="294"/>
+      <c r="H5" s="295"/>
+      <c r="I5" s="295"/>
+      <c r="J5" s="295"/>
+      <c r="K5" s="296"/>
       <c r="L5" s="173"/>
       <c r="M5" s="173">
         <v>3</v>
@@ -28537,11 +28540,11 @@
       <c r="D6" s="229"/>
       <c r="E6" s="185"/>
       <c r="F6" s="185"/>
-      <c r="G6" s="268"/>
-      <c r="H6" s="273"/>
-      <c r="I6" s="273"/>
-      <c r="J6" s="273"/>
-      <c r="K6" s="274"/>
+      <c r="G6" s="294"/>
+      <c r="H6" s="295"/>
+      <c r="I6" s="295"/>
+      <c r="J6" s="295"/>
+      <c r="K6" s="296"/>
       <c r="L6" s="173"/>
       <c r="M6" s="173">
         <v>4</v>
@@ -28579,11 +28582,11 @@
       <c r="D7" s="187"/>
       <c r="E7" s="185"/>
       <c r="F7" s="185"/>
-      <c r="G7" s="268"/>
-      <c r="H7" s="273"/>
-      <c r="I7" s="273"/>
-      <c r="J7" s="273"/>
-      <c r="K7" s="274"/>
+      <c r="G7" s="294"/>
+      <c r="H7" s="295"/>
+      <c r="I7" s="295"/>
+      <c r="J7" s="295"/>
+      <c r="K7" s="296"/>
       <c r="L7" s="173"/>
       <c r="M7" s="173">
         <v>5</v>
@@ -28621,11 +28624,11 @@
       <c r="D8" s="187"/>
       <c r="E8" s="185"/>
       <c r="F8" s="185"/>
-      <c r="G8" s="268"/>
-      <c r="H8" s="273"/>
-      <c r="I8" s="273"/>
-      <c r="J8" s="273"/>
-      <c r="K8" s="274"/>
+      <c r="G8" s="294"/>
+      <c r="H8" s="295"/>
+      <c r="I8" s="295"/>
+      <c r="J8" s="295"/>
+      <c r="K8" s="296"/>
       <c r="L8" s="173"/>
       <c r="M8" s="173">
         <v>6</v>
@@ -28663,11 +28666,11 @@
       <c r="D9" s="187"/>
       <c r="E9" s="185"/>
       <c r="F9" s="185"/>
-      <c r="G9" s="268"/>
-      <c r="H9" s="273"/>
-      <c r="I9" s="273"/>
-      <c r="J9" s="273"/>
-      <c r="K9" s="274"/>
+      <c r="G9" s="294"/>
+      <c r="H9" s="295"/>
+      <c r="I9" s="295"/>
+      <c r="J9" s="295"/>
+      <c r="K9" s="296"/>
       <c r="L9" s="173"/>
       <c r="M9" s="173">
         <v>7</v>
@@ -28705,11 +28708,11 @@
       <c r="D10" s="187"/>
       <c r="E10" s="185"/>
       <c r="F10" s="185"/>
-      <c r="G10" s="268"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="270"/>
+      <c r="G10" s="294"/>
+      <c r="H10" s="300"/>
+      <c r="I10" s="300"/>
+      <c r="J10" s="300"/>
+      <c r="K10" s="301"/>
       <c r="L10" s="173"/>
       <c r="M10" s="173">
         <v>8</v>
@@ -28747,11 +28750,11 @@
       <c r="D11" s="102"/>
       <c r="E11" s="185"/>
       <c r="F11" s="185"/>
-      <c r="G11" s="268"/>
-      <c r="H11" s="269"/>
-      <c r="I11" s="269"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="270"/>
+      <c r="G11" s="294"/>
+      <c r="H11" s="300"/>
+      <c r="I11" s="300"/>
+      <c r="J11" s="300"/>
+      <c r="K11" s="301"/>
       <c r="L11" s="173"/>
       <c r="M11" s="173">
         <v>9</v>
@@ -28789,11 +28792,11 @@
       <c r="D12" s="187"/>
       <c r="E12" s="130"/>
       <c r="F12" s="185"/>
-      <c r="G12" s="268"/>
-      <c r="H12" s="269"/>
-      <c r="I12" s="269"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="270"/>
+      <c r="G12" s="294"/>
+      <c r="H12" s="300"/>
+      <c r="I12" s="300"/>
+      <c r="J12" s="300"/>
+      <c r="K12" s="301"/>
       <c r="L12" s="173"/>
       <c r="M12" s="173">
         <v>10</v>
@@ -28831,11 +28834,11 @@
       <c r="D13" s="102"/>
       <c r="E13" s="185"/>
       <c r="F13" s="185"/>
-      <c r="G13" s="268"/>
-      <c r="H13" s="269"/>
-      <c r="I13" s="269"/>
-      <c r="J13" s="269"/>
-      <c r="K13" s="270"/>
+      <c r="G13" s="294"/>
+      <c r="H13" s="300"/>
+      <c r="I13" s="300"/>
+      <c r="J13" s="300"/>
+      <c r="K13" s="301"/>
       <c r="L13" s="173"/>
       <c r="M13" s="173">
         <v>11</v>
@@ -28873,11 +28876,11 @@
       <c r="D14" s="187"/>
       <c r="E14" s="185"/>
       <c r="F14" s="185"/>
-      <c r="G14" s="268"/>
-      <c r="H14" s="269"/>
-      <c r="I14" s="269"/>
-      <c r="J14" s="269"/>
-      <c r="K14" s="270"/>
+      <c r="G14" s="294"/>
+      <c r="H14" s="300"/>
+      <c r="I14" s="300"/>
+      <c r="J14" s="300"/>
+      <c r="K14" s="301"/>
       <c r="L14" s="173"/>
       <c r="M14" s="173">
         <v>12</v>
@@ -28915,11 +28918,11 @@
       <c r="D15" s="102"/>
       <c r="E15" s="130"/>
       <c r="F15" s="185"/>
-      <c r="G15" s="268"/>
-      <c r="H15" s="269"/>
-      <c r="I15" s="269"/>
-      <c r="J15" s="269"/>
-      <c r="K15" s="270"/>
+      <c r="G15" s="294"/>
+      <c r="H15" s="300"/>
+      <c r="I15" s="300"/>
+      <c r="J15" s="300"/>
+      <c r="K15" s="301"/>
       <c r="L15" s="173"/>
       <c r="M15" s="173">
         <v>13</v>
@@ -28957,11 +28960,11 @@
       <c r="D16" s="102"/>
       <c r="E16" s="130"/>
       <c r="F16" s="185"/>
-      <c r="G16" s="268"/>
-      <c r="H16" s="269"/>
-      <c r="I16" s="269"/>
-      <c r="J16" s="269"/>
-      <c r="K16" s="270"/>
+      <c r="G16" s="294"/>
+      <c r="H16" s="300"/>
+      <c r="I16" s="300"/>
+      <c r="J16" s="300"/>
+      <c r="K16" s="301"/>
       <c r="L16" s="173"/>
       <c r="M16" s="173">
         <v>14</v>
@@ -28999,11 +29002,11 @@
       <c r="D17" s="102"/>
       <c r="E17" s="130"/>
       <c r="F17" s="185"/>
-      <c r="G17" s="268"/>
-      <c r="H17" s="269"/>
-      <c r="I17" s="269"/>
-      <c r="J17" s="269"/>
-      <c r="K17" s="270"/>
+      <c r="G17" s="294"/>
+      <c r="H17" s="300"/>
+      <c r="I17" s="300"/>
+      <c r="J17" s="300"/>
+      <c r="K17" s="301"/>
       <c r="L17" s="173"/>
       <c r="M17" s="173">
         <v>15</v>
@@ -29041,11 +29044,11 @@
       <c r="D18" s="102"/>
       <c r="E18" s="130"/>
       <c r="F18" s="185"/>
-      <c r="G18" s="268"/>
-      <c r="H18" s="269"/>
-      <c r="I18" s="269"/>
-      <c r="J18" s="269"/>
-      <c r="K18" s="270"/>
+      <c r="G18" s="294"/>
+      <c r="H18" s="300"/>
+      <c r="I18" s="300"/>
+      <c r="J18" s="300"/>
+      <c r="K18" s="301"/>
       <c r="L18" s="173"/>
       <c r="M18" s="173">
         <v>16</v>
@@ -29083,11 +29086,11 @@
       <c r="D19" s="102"/>
       <c r="E19" s="185"/>
       <c r="F19" s="185"/>
-      <c r="G19" s="268"/>
-      <c r="H19" s="269"/>
-      <c r="I19" s="269"/>
-      <c r="J19" s="269"/>
-      <c r="K19" s="270"/>
+      <c r="G19" s="294"/>
+      <c r="H19" s="300"/>
+      <c r="I19" s="300"/>
+      <c r="J19" s="300"/>
+      <c r="K19" s="301"/>
       <c r="L19" s="173"/>
       <c r="M19" s="173">
         <v>17</v>
@@ -29125,11 +29128,11 @@
       <c r="D20" s="187"/>
       <c r="E20" s="185"/>
       <c r="F20" s="185"/>
-      <c r="G20" s="268"/>
-      <c r="H20" s="269"/>
-      <c r="I20" s="269"/>
-      <c r="J20" s="269"/>
-      <c r="K20" s="270"/>
+      <c r="G20" s="294"/>
+      <c r="H20" s="300"/>
+      <c r="I20" s="300"/>
+      <c r="J20" s="300"/>
+      <c r="K20" s="301"/>
       <c r="L20" s="173"/>
       <c r="M20" s="173">
         <v>18</v>
@@ -29167,11 +29170,11 @@
       <c r="D21" s="187"/>
       <c r="E21" s="185"/>
       <c r="F21" s="185"/>
-      <c r="G21" s="268"/>
-      <c r="H21" s="269"/>
-      <c r="I21" s="269"/>
-      <c r="J21" s="269"/>
-      <c r="K21" s="270"/>
+      <c r="G21" s="294"/>
+      <c r="H21" s="300"/>
+      <c r="I21" s="300"/>
+      <c r="J21" s="300"/>
+      <c r="K21" s="301"/>
       <c r="L21" s="173"/>
       <c r="M21" s="173">
         <v>19</v>
@@ -29209,11 +29212,11 @@
       <c r="D22" s="102"/>
       <c r="E22" s="130"/>
       <c r="F22" s="185"/>
-      <c r="G22" s="268"/>
-      <c r="H22" s="269"/>
-      <c r="I22" s="269"/>
-      <c r="J22" s="269"/>
-      <c r="K22" s="270"/>
+      <c r="G22" s="294"/>
+      <c r="H22" s="300"/>
+      <c r="I22" s="300"/>
+      <c r="J22" s="300"/>
+      <c r="K22" s="301"/>
       <c r="L22" s="173"/>
       <c r="M22" s="173">
         <v>20</v>
@@ -29251,11 +29254,11 @@
       <c r="D23" s="187"/>
       <c r="E23" s="185"/>
       <c r="F23" s="185"/>
-      <c r="G23" s="268"/>
-      <c r="H23" s="269"/>
-      <c r="I23" s="269"/>
-      <c r="J23" s="269"/>
-      <c r="K23" s="270"/>
+      <c r="G23" s="294"/>
+      <c r="H23" s="300"/>
+      <c r="I23" s="300"/>
+      <c r="J23" s="300"/>
+      <c r="K23" s="301"/>
       <c r="L23" s="173"/>
       <c r="M23" s="173">
         <v>21</v>
@@ -29335,11 +29338,11 @@
       <c r="D25" s="187"/>
       <c r="E25" s="130"/>
       <c r="F25" s="185"/>
-      <c r="G25" s="268"/>
-      <c r="H25" s="269"/>
-      <c r="I25" s="269"/>
-      <c r="J25" s="269"/>
-      <c r="K25" s="270"/>
+      <c r="G25" s="294"/>
+      <c r="H25" s="300"/>
+      <c r="I25" s="300"/>
+      <c r="J25" s="300"/>
+      <c r="K25" s="301"/>
       <c r="L25" s="173"/>
       <c r="M25" s="173">
         <v>23</v>
@@ -29377,11 +29380,11 @@
       <c r="D26" s="187"/>
       <c r="E26" s="102"/>
       <c r="F26" s="185"/>
-      <c r="G26" s="268"/>
-      <c r="H26" s="269"/>
-      <c r="I26" s="269"/>
-      <c r="J26" s="269"/>
-      <c r="K26" s="270"/>
+      <c r="G26" s="294"/>
+      <c r="H26" s="300"/>
+      <c r="I26" s="300"/>
+      <c r="J26" s="300"/>
+      <c r="K26" s="301"/>
       <c r="L26" s="173"/>
       <c r="M26" s="173">
         <v>24</v>
@@ -29419,11 +29422,11 @@
       <c r="D27" s="187"/>
       <c r="E27" s="130"/>
       <c r="F27" s="185"/>
-      <c r="G27" s="268"/>
-      <c r="H27" s="269"/>
-      <c r="I27" s="269"/>
-      <c r="J27" s="269"/>
-      <c r="K27" s="270"/>
+      <c r="G27" s="294"/>
+      <c r="H27" s="300"/>
+      <c r="I27" s="300"/>
+      <c r="J27" s="300"/>
+      <c r="K27" s="301"/>
       <c r="L27" s="173"/>
       <c r="M27" s="173">
         <v>25</v>
@@ -29461,11 +29464,11 @@
       <c r="D28" s="102"/>
       <c r="E28" s="130"/>
       <c r="F28" s="185"/>
-      <c r="G28" s="268"/>
-      <c r="H28" s="269"/>
-      <c r="I28" s="269"/>
-      <c r="J28" s="269"/>
-      <c r="K28" s="270"/>
+      <c r="G28" s="294"/>
+      <c r="H28" s="300"/>
+      <c r="I28" s="300"/>
+      <c r="J28" s="300"/>
+      <c r="K28" s="301"/>
       <c r="L28" s="173"/>
       <c r="M28" s="173">
         <v>26</v>
@@ -29503,11 +29506,11 @@
       <c r="D29" s="102"/>
       <c r="E29" s="185"/>
       <c r="F29" s="185"/>
-      <c r="G29" s="268"/>
-      <c r="H29" s="269"/>
-      <c r="I29" s="269"/>
-      <c r="J29" s="269"/>
-      <c r="K29" s="270"/>
+      <c r="G29" s="294"/>
+      <c r="H29" s="300"/>
+      <c r="I29" s="300"/>
+      <c r="J29" s="300"/>
+      <c r="K29" s="301"/>
       <c r="L29" s="173"/>
       <c r="M29" s="173">
         <v>27</v>
@@ -29545,11 +29548,11 @@
       <c r="D30" s="187"/>
       <c r="E30" s="185"/>
       <c r="F30" s="185"/>
-      <c r="G30" s="268"/>
-      <c r="H30" s="269"/>
-      <c r="I30" s="269"/>
-      <c r="J30" s="269"/>
-      <c r="K30" s="270"/>
+      <c r="G30" s="294"/>
+      <c r="H30" s="300"/>
+      <c r="I30" s="300"/>
+      <c r="J30" s="300"/>
+      <c r="K30" s="301"/>
       <c r="L30" s="173"/>
       <c r="M30" s="173">
         <v>28</v>
@@ -29587,11 +29590,11 @@
       <c r="D31" s="187"/>
       <c r="E31" s="130"/>
       <c r="F31" s="185"/>
-      <c r="G31" s="268"/>
-      <c r="H31" s="269"/>
-      <c r="I31" s="269"/>
-      <c r="J31" s="269"/>
-      <c r="K31" s="270"/>
+      <c r="G31" s="294"/>
+      <c r="H31" s="300"/>
+      <c r="I31" s="300"/>
+      <c r="J31" s="300"/>
+      <c r="K31" s="301"/>
       <c r="L31" s="173"/>
       <c r="M31" s="173">
         <v>29</v>
@@ -29629,11 +29632,11 @@
       <c r="D32" s="102"/>
       <c r="E32" s="185"/>
       <c r="F32" s="185"/>
-      <c r="G32" s="268"/>
-      <c r="H32" s="269"/>
-      <c r="I32" s="269"/>
-      <c r="J32" s="269"/>
-      <c r="K32" s="270"/>
+      <c r="G32" s="294"/>
+      <c r="H32" s="300"/>
+      <c r="I32" s="300"/>
+      <c r="J32" s="300"/>
+      <c r="K32" s="301"/>
       <c r="L32" s="173"/>
       <c r="M32" s="173">
         <v>30</v>
@@ -29671,11 +29674,11 @@
       <c r="D33" s="173"/>
       <c r="E33" s="130"/>
       <c r="F33" s="185"/>
-      <c r="G33" s="268"/>
-      <c r="H33" s="269"/>
-      <c r="I33" s="269"/>
-      <c r="J33" s="269"/>
-      <c r="K33" s="270"/>
+      <c r="G33" s="294"/>
+      <c r="H33" s="300"/>
+      <c r="I33" s="300"/>
+      <c r="J33" s="300"/>
+      <c r="K33" s="301"/>
       <c r="L33" s="173"/>
       <c r="M33" s="173">
         <v>31</v>
@@ -29711,11 +29714,11 @@
       <c r="D34" s="102"/>
       <c r="E34" s="102"/>
       <c r="F34" s="185"/>
-      <c r="G34" s="268"/>
-      <c r="H34" s="269"/>
-      <c r="I34" s="269"/>
-      <c r="J34" s="269"/>
-      <c r="K34" s="270"/>
+      <c r="G34" s="294"/>
+      <c r="H34" s="300"/>
+      <c r="I34" s="300"/>
+      <c r="J34" s="300"/>
+      <c r="K34" s="301"/>
       <c r="L34" s="173"/>
       <c r="M34" s="173"/>
       <c r="N34" s="173"/>
@@ -29767,11 +29770,11 @@
       <c r="D35" s="102"/>
       <c r="E35" s="130"/>
       <c r="F35" s="185"/>
-      <c r="G35" s="268"/>
-      <c r="H35" s="269"/>
-      <c r="I35" s="269"/>
-      <c r="J35" s="269"/>
-      <c r="K35" s="270"/>
+      <c r="G35" s="294"/>
+      <c r="H35" s="300"/>
+      <c r="I35" s="300"/>
+      <c r="J35" s="300"/>
+      <c r="K35" s="301"/>
       <c r="L35" s="173"/>
       <c r="M35" s="173"/>
       <c r="N35" s="190">
@@ -29809,11 +29812,11 @@
       <c r="D36" s="192"/>
       <c r="E36" s="192"/>
       <c r="F36" s="193"/>
-      <c r="G36" s="265"/>
-      <c r="H36" s="266"/>
-      <c r="I36" s="266"/>
-      <c r="J36" s="266"/>
-      <c r="K36" s="267"/>
+      <c r="G36" s="302"/>
+      <c r="H36" s="303"/>
+      <c r="I36" s="303"/>
+      <c r="J36" s="303"/>
+      <c r="K36" s="304"/>
       <c r="L36" s="173"/>
       <c r="M36" s="173"/>
       <c r="N36" s="173"/>
@@ -37000,16 +37003,18 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
     <mergeCell ref="G10:K10"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="G12:K12"/>
@@ -37024,18 +37029,16 @@
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="G22:K22"/>
-    <mergeCell ref="G36:K36"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" prompt="INPUT TICKET NUMBER - Please input the ticket number. Use &quot;/&quot; to separate multiple ticket numbers." sqref="AB22:AB28 X3:AA33 C22:C28 AB9:AB17 C9:C17" xr:uid="{6EBA5DD2-9520-1C44-B6DD-78BB8475944E}">

</xml_diff>